<commit_message>
Replaced the line chart dataset
</commit_message>
<xml_diff>
--- a/Assignment_1/Data_sets/Line_Chart_DataSet.xlsx
+++ b/Assignment_1/Data_sets/Line_Chart_DataSet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CherukuR\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\Applied_Data_Science\Assignment_1\Data_sets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1728A51-0590-445E-95F7-1A46CDB031A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33F93B0-D11E-431F-8199-3270541A735B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Neonatal_Deaths_Data" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -506,7 +506,7 @@
         <v>602468</v>
       </c>
       <c r="D8">
-        <v>84367</v>
+        <v>84368</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>